<commit_message>
Changes filled_template fixture attributes to valid MODS
</commit_message>
<xml_diff>
--- a/spec/fixtures/filled_template_20160711.xlsx
+++ b/spec/fixtures/filled_template_20160711.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arcadia\Box Sync\GitHub\modsulator\spec\fixtures\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arcadia\Box Sync\Projects\Digital collections\modsulator\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -85,7 +85,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2275" uniqueCount="1125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2275" uniqueCount="1139">
   <si>
     <t>Identification</t>
   </si>
@@ -3460,6 +3460,48 @@
   </si>
   <si>
     <t>rc:scriptOfCataloging2Term</t>
+  </si>
+  <si>
+    <t>abbreviated</t>
+  </si>
+  <si>
+    <t>personal</t>
+  </si>
+  <si>
+    <t>primary</t>
+  </si>
+  <si>
+    <t>text</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>w3cdtf</t>
+  </si>
+  <si>
+    <t>approximate</t>
+  </si>
+  <si>
+    <t>start</t>
+  </si>
+  <si>
+    <t>marcgac</t>
+  </si>
+  <si>
+    <t>continuing</t>
+  </si>
+  <si>
+    <t>rfc3066</t>
+  </si>
+  <si>
+    <t>access</t>
+  </si>
+  <si>
+    <t>born digital</t>
+  </si>
+  <si>
+    <t>preceding</t>
   </si>
 </sst>
 </file>
@@ -4161,9 +4203,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AOZ3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="ANP1" workbookViewId="0">
-      <selection activeCell="AOM4" sqref="AOM4"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -8770,7 +8810,7 @@
         <v>1118</v>
       </c>
     </row>
-    <row r="3" spans="1:1092" s="53" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1092" s="53" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="48">
         <v>123</v>
       </c>
@@ -8817,7 +8857,7 @@
         <v>102</v>
       </c>
       <c r="P3" s="49" t="s">
-        <v>103</v>
+        <v>1125</v>
       </c>
       <c r="Q3" s="50" t="s">
         <v>104</v>
@@ -8863,7 +8903,7 @@
       </c>
       <c r="AE3" s="51"/>
       <c r="AF3" s="49" t="s">
-        <v>118</v>
+        <v>1125</v>
       </c>
       <c r="AG3" s="50" t="s">
         <v>119</v>
@@ -8912,10 +8952,10 @@
         <v>133</v>
       </c>
       <c r="AW3" s="48" t="s">
-        <v>134</v>
+        <v>1126</v>
       </c>
       <c r="AX3" s="48" t="s">
-        <v>135</v>
+        <v>1127</v>
       </c>
       <c r="AY3" s="48" t="s">
         <v>136</v>
@@ -8990,7 +9030,7 @@
         <v>159</v>
       </c>
       <c r="BW3" s="48" t="s">
-        <v>160</v>
+        <v>1126</v>
       </c>
       <c r="BX3" s="48" t="s">
         <v>161</v>
@@ -9068,7 +9108,7 @@
         <v>184</v>
       </c>
       <c r="CY3" s="48" t="s">
-        <v>185</v>
+        <v>1126</v>
       </c>
       <c r="CZ3" s="48" t="s">
         <v>186</v>
@@ -9146,7 +9186,7 @@
         <v>209</v>
       </c>
       <c r="EA3" s="48" t="s">
-        <v>210</v>
+        <v>1126</v>
       </c>
       <c r="EB3" s="48" t="s">
         <v>211</v>
@@ -9224,7 +9264,7 @@
         <v>234</v>
       </c>
       <c r="FC3" s="48" t="s">
-        <v>235</v>
+        <v>1126</v>
       </c>
       <c r="FD3" s="48" t="s">
         <v>236</v>
@@ -9299,17 +9339,17 @@
       <c r="GB3" s="50"/>
       <c r="GC3" s="51"/>
       <c r="GD3" s="50" t="s">
-        <v>259</v>
+        <v>1128</v>
       </c>
       <c r="GE3" s="54" t="s">
-        <v>260</v>
+        <v>1129</v>
       </c>
       <c r="GF3" s="50" t="s">
-        <v>261</v>
+        <v>1128</v>
       </c>
       <c r="GG3" s="51"/>
       <c r="GH3" s="55" t="s">
-        <v>262</v>
+        <v>1128</v>
       </c>
       <c r="GI3" s="51"/>
       <c r="GJ3" s="56" t="s">
@@ -9363,115 +9403,115 @@
         <v>278</v>
       </c>
       <c r="HB3" s="50" t="s">
-        <v>279</v>
+        <v>1129</v>
       </c>
       <c r="HC3" s="50" t="s">
-        <v>280</v>
+        <v>1130</v>
       </c>
       <c r="HD3" s="50" t="s">
-        <v>281</v>
+        <v>1131</v>
       </c>
       <c r="HE3" s="50" t="s">
-        <v>282</v>
+        <v>1132</v>
       </c>
       <c r="HF3" s="50" t="s">
         <v>283</v>
       </c>
       <c r="HG3" s="50" t="s">
-        <v>284</v>
+        <v>1131</v>
       </c>
       <c r="HH3" s="50" t="s">
-        <v>285</v>
+        <v>1132</v>
       </c>
       <c r="HI3" s="50" t="s">
         <v>286</v>
       </c>
       <c r="HJ3" s="50" t="s">
-        <v>287</v>
+        <v>1129</v>
       </c>
       <c r="HK3" s="50" t="s">
-        <v>288</v>
+        <v>1130</v>
       </c>
       <c r="HL3" s="50" t="s">
-        <v>289</v>
+        <v>1131</v>
       </c>
       <c r="HM3" s="50" t="s">
-        <v>290</v>
+        <v>1132</v>
       </c>
       <c r="HN3" s="50" t="s">
         <v>291</v>
       </c>
       <c r="HO3" s="50" t="s">
-        <v>292</v>
+        <v>1131</v>
       </c>
       <c r="HP3" s="50" t="s">
-        <v>293</v>
+        <v>1132</v>
       </c>
       <c r="HQ3" s="50" t="s">
         <v>294</v>
       </c>
       <c r="HR3" s="50" t="s">
-        <v>295</v>
+        <v>1129</v>
       </c>
       <c r="HS3" s="50" t="s">
-        <v>296</v>
+        <v>1130</v>
       </c>
       <c r="HT3" s="50" t="s">
-        <v>297</v>
+        <v>1131</v>
       </c>
       <c r="HU3" s="50" t="s">
-        <v>298</v>
+        <v>1132</v>
       </c>
       <c r="HV3" s="50" t="s">
         <v>299</v>
       </c>
       <c r="HW3" s="50" t="s">
-        <v>300</v>
+        <v>1131</v>
       </c>
       <c r="HX3" s="50" t="s">
-        <v>301</v>
+        <v>1132</v>
       </c>
       <c r="HY3" s="50" t="s">
         <v>302</v>
       </c>
       <c r="HZ3" s="50" t="s">
-        <v>303</v>
+        <v>1129</v>
       </c>
       <c r="IA3" s="50" t="s">
-        <v>304</v>
+        <v>1130</v>
       </c>
       <c r="IB3" s="50" t="s">
-        <v>305</v>
+        <v>1131</v>
       </c>
       <c r="IC3" s="50" t="s">
-        <v>306</v>
+        <v>1132</v>
       </c>
       <c r="ID3" s="50" t="s">
         <v>307</v>
       </c>
       <c r="IE3" s="50" t="s">
-        <v>308</v>
+        <v>1131</v>
       </c>
       <c r="IF3" s="50" t="s">
-        <v>309</v>
+        <v>1132</v>
       </c>
       <c r="IG3" s="50" t="s">
         <v>310</v>
       </c>
       <c r="IH3" s="50" t="s">
-        <v>311</v>
+        <v>1129</v>
       </c>
       <c r="II3" s="50" t="s">
         <v>312</v>
       </c>
       <c r="IJ3" s="50" t="s">
-        <v>313</v>
+        <v>1130</v>
       </c>
       <c r="IK3" s="50" t="s">
-        <v>314</v>
+        <v>1131</v>
       </c>
       <c r="IL3" s="50" t="s">
-        <v>315</v>
+        <v>1132</v>
       </c>
       <c r="IM3" s="50" t="s">
         <v>316</v>
@@ -9483,10 +9523,10 @@
         <v>318</v>
       </c>
       <c r="IP3" s="50" t="s">
-        <v>319</v>
+        <v>1131</v>
       </c>
       <c r="IQ3" s="50" t="s">
-        <v>320</v>
+        <v>1132</v>
       </c>
       <c r="IR3" s="49" t="s">
         <v>321</v>
@@ -9516,7 +9556,7 @@
         <v>329</v>
       </c>
       <c r="JA3" s="48" t="s">
-        <v>330</v>
+        <v>1133</v>
       </c>
       <c r="JB3" s="48" t="s">
         <v>331</v>
@@ -9528,121 +9568,121 @@
         <v>333</v>
       </c>
       <c r="JE3" s="48" t="s">
-        <v>334</v>
+        <v>1134</v>
       </c>
       <c r="JF3" s="49" t="s">
         <v>335</v>
       </c>
       <c r="JG3" s="50" t="s">
-        <v>336</v>
+        <v>1129</v>
       </c>
       <c r="JH3" s="50" t="s">
-        <v>337</v>
+        <v>1130</v>
       </c>
       <c r="JI3" s="50" t="s">
-        <v>338</v>
+        <v>1131</v>
       </c>
       <c r="JJ3" s="50" t="s">
-        <v>339</v>
+        <v>1132</v>
       </c>
       <c r="JK3" s="50" t="s">
         <v>340</v>
       </c>
       <c r="JL3" s="50" t="s">
-        <v>341</v>
+        <v>1131</v>
       </c>
       <c r="JM3" s="50" t="s">
-        <v>342</v>
+        <v>1132</v>
       </c>
       <c r="JN3" s="50" t="s">
         <v>343</v>
       </c>
       <c r="JO3" s="50" t="s">
-        <v>344</v>
+        <v>1129</v>
       </c>
       <c r="JP3" s="50" t="s">
-        <v>345</v>
+        <v>1130</v>
       </c>
       <c r="JQ3" s="50" t="s">
-        <v>346</v>
+        <v>1131</v>
       </c>
       <c r="JR3" s="50" t="s">
-        <v>347</v>
+        <v>1132</v>
       </c>
       <c r="JS3" s="50" t="s">
         <v>348</v>
       </c>
       <c r="JT3" s="50" t="s">
-        <v>349</v>
+        <v>1131</v>
       </c>
       <c r="JU3" s="50" t="s">
-        <v>350</v>
+        <v>1132</v>
       </c>
       <c r="JV3" s="50" t="s">
         <v>351</v>
       </c>
       <c r="JW3" s="50" t="s">
-        <v>352</v>
+        <v>1129</v>
       </c>
       <c r="JX3" s="50" t="s">
-        <v>353</v>
+        <v>1130</v>
       </c>
       <c r="JY3" s="50" t="s">
-        <v>354</v>
+        <v>1131</v>
       </c>
       <c r="JZ3" s="50" t="s">
-        <v>355</v>
+        <v>1132</v>
       </c>
       <c r="KA3" s="50" t="s">
         <v>356</v>
       </c>
       <c r="KB3" s="50" t="s">
-        <v>357</v>
+        <v>1131</v>
       </c>
       <c r="KC3" s="50" t="s">
-        <v>358</v>
+        <v>1132</v>
       </c>
       <c r="KD3" s="50" t="s">
         <v>359</v>
       </c>
       <c r="KE3" s="50" t="s">
-        <v>360</v>
+        <v>1129</v>
       </c>
       <c r="KF3" s="50" t="s">
-        <v>361</v>
+        <v>1130</v>
       </c>
       <c r="KG3" s="50" t="s">
-        <v>362</v>
+        <v>1131</v>
       </c>
       <c r="KH3" s="50" t="s">
-        <v>363</v>
+        <v>1132</v>
       </c>
       <c r="KI3" s="50" t="s">
         <v>364</v>
       </c>
       <c r="KJ3" s="50" t="s">
-        <v>365</v>
+        <v>1131</v>
       </c>
       <c r="KK3" s="50" t="s">
-        <v>366</v>
+        <v>1132</v>
       </c>
       <c r="KL3" s="50" t="s">
         <v>367</v>
       </c>
       <c r="KM3" s="50" t="s">
-        <v>368</v>
+        <v>1129</v>
       </c>
       <c r="KN3" s="50" t="s">
         <v>369</v>
       </c>
       <c r="KO3" s="50" t="s">
-        <v>370</v>
+        <v>1130</v>
       </c>
       <c r="KP3" s="50" t="s">
-        <v>371</v>
+        <v>1131</v>
       </c>
       <c r="KQ3" s="50" t="s">
-        <v>372</v>
+        <v>1132</v>
       </c>
       <c r="KR3" s="50" t="s">
         <v>373</v>
@@ -9654,10 +9694,10 @@
         <v>375</v>
       </c>
       <c r="KU3" s="50" t="s">
-        <v>376</v>
+        <v>1131</v>
       </c>
       <c r="KV3" s="50" t="s">
-        <v>377</v>
+        <v>1132</v>
       </c>
       <c r="KW3" s="50" t="s">
         <v>378</v>
@@ -9687,7 +9727,7 @@
         <v>386</v>
       </c>
       <c r="LF3" s="48" t="s">
-        <v>387</v>
+        <v>1133</v>
       </c>
       <c r="LG3" s="48" t="s">
         <v>388</v>
@@ -9699,7 +9739,7 @@
         <v>390</v>
       </c>
       <c r="LJ3" s="48" t="s">
-        <v>391</v>
+        <v>1134</v>
       </c>
       <c r="LK3" s="48"/>
       <c r="LL3" s="56" t="s">
@@ -9709,7 +9749,7 @@
         <v>393</v>
       </c>
       <c r="LN3" s="50" t="s">
-        <v>394</v>
+        <v>1135</v>
       </c>
       <c r="LO3" s="50" t="s">
         <v>395</v>
@@ -9724,7 +9764,7 @@
         <v>398</v>
       </c>
       <c r="LS3" s="48" t="s">
-        <v>399</v>
+        <v>1135</v>
       </c>
       <c r="LT3" s="48" t="s">
         <v>400</v>
@@ -9740,7 +9780,7 @@
         <v>403</v>
       </c>
       <c r="LY3" s="48" t="s">
-        <v>404</v>
+        <v>1135</v>
       </c>
       <c r="LZ3" s="48" t="s">
         <v>405</v>
@@ -9765,10 +9805,10 @@
         <v>411</v>
       </c>
       <c r="MH3" s="48" t="s">
-        <v>412</v>
+        <v>1136</v>
       </c>
       <c r="MI3" s="48" t="s">
-        <v>413</v>
+        <v>1137</v>
       </c>
       <c r="MJ3" s="48" t="s">
         <v>414</v>
@@ -9939,10 +9979,10 @@
         <v>469</v>
       </c>
       <c r="ON3" s="48" t="s">
-        <v>470</v>
+        <v>1136</v>
       </c>
       <c r="OO3" s="48" t="s">
-        <v>471</v>
+        <v>1137</v>
       </c>
       <c r="OP3" s="57" t="s">
         <v>472</v>
@@ -9976,10 +10016,10 @@
         <v>481</v>
       </c>
       <c r="PA3" s="48" t="s">
-        <v>482</v>
+        <v>1136</v>
       </c>
       <c r="PB3" s="48" t="s">
-        <v>483</v>
+        <v>1137</v>
       </c>
       <c r="PC3" s="57" t="s">
         <v>484</v>
@@ -10152,7 +10192,7 @@
         <v>538</v>
       </c>
       <c r="RK3" s="48" t="s">
-        <v>539</v>
+        <v>1126</v>
       </c>
       <c r="RL3" s="48" t="s">
         <v>540</v>
@@ -10176,7 +10216,7 @@
         <v>546</v>
       </c>
       <c r="RS3" s="48" t="s">
-        <v>547</v>
+        <v>1125</v>
       </c>
       <c r="RT3" s="48" t="s">
         <v>548</v>
@@ -10281,7 +10321,7 @@
         <v>581</v>
       </c>
       <c r="TB3" s="48" t="s">
-        <v>582</v>
+        <v>1126</v>
       </c>
       <c r="TC3" s="48" t="s">
         <v>583</v>
@@ -10305,7 +10345,7 @@
         <v>589</v>
       </c>
       <c r="TJ3" s="48" t="s">
-        <v>590</v>
+        <v>1125</v>
       </c>
       <c r="TK3" s="48" t="s">
         <v>591</v>
@@ -10411,7 +10451,7 @@
         <v>624</v>
       </c>
       <c r="UT3" s="48" t="s">
-        <v>625</v>
+        <v>1126</v>
       </c>
       <c r="UU3" s="48" t="s">
         <v>626</v>
@@ -10435,7 +10475,7 @@
         <v>632</v>
       </c>
       <c r="VB3" s="48" t="s">
-        <v>633</v>
+        <v>1125</v>
       </c>
       <c r="VC3" s="48" t="s">
         <v>634</v>
@@ -10541,7 +10581,7 @@
         <v>667</v>
       </c>
       <c r="WL3" s="48" t="s">
-        <v>668</v>
+        <v>1126</v>
       </c>
       <c r="WM3" s="48" t="s">
         <v>669</v>
@@ -10565,7 +10605,7 @@
         <v>675</v>
       </c>
       <c r="WT3" s="48" t="s">
-        <v>676</v>
+        <v>1125</v>
       </c>
       <c r="WU3" s="48" t="s">
         <v>677</v>
@@ -10671,7 +10711,7 @@
         <v>710</v>
       </c>
       <c r="YD3" s="48" t="s">
-        <v>711</v>
+        <v>1126</v>
       </c>
       <c r="YE3" s="48" t="s">
         <v>712</v>
@@ -10695,7 +10735,7 @@
         <v>718</v>
       </c>
       <c r="YL3" s="48" t="s">
-        <v>719</v>
+        <v>1125</v>
       </c>
       <c r="YM3" s="48" t="s">
         <v>720</v>
@@ -11355,7 +11395,7 @@
       </c>
       <c r="AHC3" s="64"/>
       <c r="AHD3" s="53" t="s">
-        <v>936</v>
+        <v>1138</v>
       </c>
       <c r="AHE3" s="53" t="s">
         <v>937</v>
@@ -11367,7 +11407,7 @@
         <v>939</v>
       </c>
       <c r="AHH3" s="53" t="s">
-        <v>940</v>
+        <v>1126</v>
       </c>
       <c r="AHI3" s="53" t="s">
         <v>941</v>
@@ -11416,49 +11456,49 @@
         <v>955</v>
       </c>
       <c r="AHY3" s="50" t="s">
-        <v>956</v>
+        <v>1129</v>
       </c>
       <c r="AHZ3" s="50" t="s">
-        <v>957</v>
+        <v>1130</v>
       </c>
       <c r="AIA3" s="50" t="s">
-        <v>958</v>
+        <v>1131</v>
       </c>
       <c r="AIB3" s="50" t="s">
-        <v>959</v>
+        <v>1132</v>
       </c>
       <c r="AIC3" s="50" t="s">
         <v>960</v>
       </c>
       <c r="AID3" s="50" t="s">
-        <v>961</v>
+        <v>1131</v>
       </c>
       <c r="AIE3" s="50" t="s">
-        <v>962</v>
+        <v>1132</v>
       </c>
       <c r="AIF3" s="50" t="s">
         <v>963</v>
       </c>
       <c r="AIG3" s="50" t="s">
-        <v>964</v>
+        <v>1129</v>
       </c>
       <c r="AIH3" s="50" t="s">
-        <v>965</v>
+        <v>1130</v>
       </c>
       <c r="AII3" s="50" t="s">
-        <v>966</v>
+        <v>1131</v>
       </c>
       <c r="AIJ3" s="50" t="s">
-        <v>967</v>
+        <v>1132</v>
       </c>
       <c r="AIK3" s="50" t="s">
         <v>968</v>
       </c>
       <c r="AIL3" s="48" t="s">
-        <v>969</v>
+        <v>1131</v>
       </c>
       <c r="AIM3" s="48" t="s">
-        <v>970</v>
+        <v>1132</v>
       </c>
       <c r="AIN3" s="49" t="s">
         <v>971</v>
@@ -11470,7 +11510,7 @@
         <v>973</v>
       </c>
       <c r="AIQ3" s="48" t="s">
-        <v>974</v>
+        <v>1133</v>
       </c>
       <c r="AIR3" s="48" t="s">
         <v>975</v>
@@ -11510,7 +11550,7 @@
       </c>
       <c r="AJF3" s="64"/>
       <c r="AJG3" s="53" t="s">
-        <v>986</v>
+        <v>1138</v>
       </c>
       <c r="AJH3" s="53" t="s">
         <v>987</v>
@@ -11522,7 +11562,7 @@
         <v>989</v>
       </c>
       <c r="AJK3" s="53" t="s">
-        <v>990</v>
+        <v>1126</v>
       </c>
       <c r="AJL3" s="53" t="s">
         <v>991</v>
@@ -11571,49 +11611,49 @@
         <v>1005</v>
       </c>
       <c r="AKB3" s="50" t="s">
-        <v>1006</v>
+        <v>1129</v>
       </c>
       <c r="AKC3" s="50" t="s">
-        <v>1007</v>
+        <v>1130</v>
       </c>
       <c r="AKD3" s="50" t="s">
-        <v>1008</v>
+        <v>1131</v>
       </c>
       <c r="AKE3" s="50" t="s">
-        <v>1009</v>
+        <v>1132</v>
       </c>
       <c r="AKF3" s="50" t="s">
         <v>1010</v>
       </c>
       <c r="AKG3" s="50" t="s">
-        <v>1011</v>
+        <v>1131</v>
       </c>
       <c r="AKH3" s="50" t="s">
-        <v>1012</v>
+        <v>1132</v>
       </c>
       <c r="AKI3" s="50" t="s">
         <v>1013</v>
       </c>
       <c r="AKJ3" s="50" t="s">
-        <v>1014</v>
+        <v>1129</v>
       </c>
       <c r="AKK3" s="50" t="s">
-        <v>1015</v>
+        <v>1130</v>
       </c>
       <c r="AKL3" s="50" t="s">
-        <v>1016</v>
+        <v>1131</v>
       </c>
       <c r="AKM3" s="50" t="s">
-        <v>1017</v>
+        <v>1132</v>
       </c>
       <c r="AKN3" s="50" t="s">
         <v>1018</v>
       </c>
       <c r="AKO3" s="48" t="s">
-        <v>1019</v>
+        <v>1131</v>
       </c>
       <c r="AKP3" s="48" t="s">
-        <v>1020</v>
+        <v>1132</v>
       </c>
       <c r="AKQ3" s="49" t="s">
         <v>1021</v>
@@ -11625,7 +11665,7 @@
         <v>1023</v>
       </c>
       <c r="AKT3" s="48" t="s">
-        <v>1024</v>
+        <v>1133</v>
       </c>
       <c r="AKU3" s="48" t="s">
         <v>1025</v>
@@ -11666,7 +11706,7 @@
       <c r="ALI3" s="64"/>
       <c r="ALJ3" s="65"/>
       <c r="ALK3" s="53" t="s">
-        <v>1036</v>
+        <v>1138</v>
       </c>
       <c r="ALL3" s="53" t="s">
         <v>1037</v>
@@ -11678,7 +11718,7 @@
         <v>1039</v>
       </c>
       <c r="ALO3" s="53" t="s">
-        <v>1040</v>
+        <v>1126</v>
       </c>
       <c r="ALP3" s="53" t="s">
         <v>1041</v>
@@ -11727,49 +11767,49 @@
         <v>1055</v>
       </c>
       <c r="AMF3" s="50" t="s">
-        <v>1056</v>
+        <v>1129</v>
       </c>
       <c r="AMG3" s="50" t="s">
-        <v>1057</v>
+        <v>1130</v>
       </c>
       <c r="AMH3" s="50" t="s">
-        <v>1058</v>
+        <v>1131</v>
       </c>
       <c r="AMI3" s="50" t="s">
-        <v>1059</v>
+        <v>1132</v>
       </c>
       <c r="AMJ3" s="50" t="s">
         <v>1060</v>
       </c>
       <c r="AMK3" s="50" t="s">
-        <v>1061</v>
+        <v>1131</v>
       </c>
       <c r="AML3" s="50" t="s">
-        <v>1062</v>
+        <v>1132</v>
       </c>
       <c r="AMM3" s="50" t="s">
         <v>1063</v>
       </c>
       <c r="AMN3" s="50" t="s">
-        <v>1064</v>
+        <v>1129</v>
       </c>
       <c r="AMO3" s="50" t="s">
-        <v>1065</v>
+        <v>1130</v>
       </c>
       <c r="AMP3" s="50" t="s">
-        <v>1066</v>
+        <v>1131</v>
       </c>
       <c r="AMQ3" s="50" t="s">
-        <v>1067</v>
+        <v>1132</v>
       </c>
       <c r="AMR3" s="50" t="s">
         <v>1068</v>
       </c>
       <c r="AMS3" s="48" t="s">
-        <v>1069</v>
+        <v>1131</v>
       </c>
       <c r="AMT3" s="48" t="s">
-        <v>1070</v>
+        <v>1132</v>
       </c>
       <c r="AMU3" s="49" t="s">
         <v>1071</v>
@@ -11781,7 +11821,7 @@
         <v>1073</v>
       </c>
       <c r="AMX3" s="48" t="s">
-        <v>1074</v>
+        <v>1133</v>
       </c>
       <c r="AMY3" s="48" t="s">
         <v>1075</v>
@@ -11845,13 +11885,13 @@
         <v>1093</v>
       </c>
       <c r="ANX3" s="63" t="s">
-        <v>1094</v>
+        <v>1127</v>
       </c>
       <c r="ANY3" s="63" t="s">
         <v>1121</v>
       </c>
       <c r="ANZ3" s="63" t="s">
-        <v>1095</v>
+        <v>1135</v>
       </c>
       <c r="AOA3" s="53" t="s">
         <v>1096</v>
@@ -11881,7 +11921,7 @@
         <v>1123</v>
       </c>
       <c r="AOJ3" s="53" t="s">
-        <v>1103</v>
+        <v>1135</v>
       </c>
       <c r="AOK3" s="53" t="s">
         <v>1104</v>

</xml_diff>